<commit_message>
sub folder, type of material, stamp of doc
</commit_message>
<xml_diff>
--- a/default_attributes.xlsx
+++ b/default_attributes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\demidov_ai\Documents\Демидов\Питон\ИР_эксель2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\demidov_ai\Documents\Демидов\Питон\excel_neosintez_integration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{594BF0C3-4CBB-413A-ACC1-230E45CB19AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7910976-5AA8-4381-8154-2B5DC386C67F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{ACD5EDCE-5462-4D4A-8670-E1A96D14B552}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{ACD5EDCE-5462-4D4A-8670-E1A96D14B552}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="112">
   <si>
     <t>id</t>
   </si>
@@ -325,6 +325,51 @@
   </si>
   <si>
     <t>9b1bdb78-d770-e911-8115-817c3f53a992</t>
+  </si>
+  <si>
+    <t>folder</t>
+  </si>
+  <si>
+    <t>class</t>
+  </si>
+  <si>
+    <t>df0921c1-f46f-e911-8115-817c3f53a992</t>
+  </si>
+  <si>
+    <t>0e1d8277-d859-e911-8115-817c3f53a992</t>
+  </si>
+  <si>
+    <t>c7ec82e0-f360-e911-8115-817c3f53a992</t>
+  </si>
+  <si>
+    <t>532d2888-3582-ec11-911c-005056b6948b</t>
+  </si>
+  <si>
+    <t>^(\S*)\s</t>
+  </si>
+  <si>
+    <t>regexp</t>
+  </si>
+  <si>
+    <t>regexp_name</t>
+  </si>
+  <si>
+    <t>№ поз. По ГП</t>
+  </si>
+  <si>
+    <t>Тип материала</t>
+  </si>
+  <si>
+    <t>52ad3a8a-3382-ec11-911c-005056b6948b</t>
+  </si>
+  <si>
+    <t>708c334d-e78a-ec11-911c-005056b6948b</t>
+  </si>
+  <si>
+    <t>7e2318df-0fe9-e911-80cf-9706d383f138</t>
+  </si>
+  <si>
+    <t>^.{0,5}?\.?(\S?\d+(\.\d)?)</t>
   </si>
 </sst>
 </file>
@@ -361,9 +406,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -678,10 +724,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01C59750-CE11-4137-A397-5E625D311B92}">
-  <dimension ref="A1:C48"/>
+  <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -689,9 +735,13 @@
     <col min="1" max="1" width="36.77734375" customWidth="1"/>
     <col min="2" max="2" width="16.21875" customWidth="1"/>
     <col min="3" max="3" width="35.5546875" customWidth="1"/>
+    <col min="4" max="4" width="36.109375" customWidth="1"/>
+    <col min="5" max="5" width="36.33203125" customWidth="1"/>
+    <col min="6" max="6" width="21.21875" customWidth="1"/>
+    <col min="7" max="7" width="12.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -701,8 +751,20 @@
       <c r="C1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -713,7 +775,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -724,7 +786,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -735,7 +797,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -746,7 +808,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -757,7 +819,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -768,7 +830,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -779,7 +841,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -790,7 +852,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -801,7 +863,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -812,7 +874,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -823,7 +885,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>46</v>
       </c>
@@ -834,7 +896,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>48</v>
       </c>
@@ -845,7 +907,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>50</v>
       </c>
@@ -856,7 +918,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>52</v>
       </c>
@@ -1043,7 +1105,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>76</v>
       </c>
@@ -1054,7 +1116,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>78</v>
       </c>
@@ -1065,7 +1127,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>80</v>
       </c>
@@ -1076,7 +1138,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>82</v>
       </c>
@@ -1087,7 +1149,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>34</v>
       </c>
@@ -1098,7 +1160,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -1109,7 +1171,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -1120,7 +1182,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>40</v>
       </c>
@@ -1131,7 +1193,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>42</v>
       </c>
@@ -1142,7 +1204,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>86</v>
       </c>
@@ -1153,7 +1215,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>88</v>
       </c>
@@ -1164,7 +1226,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>90</v>
       </c>
@@ -1175,7 +1237,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>92</v>
       </c>
@@ -1186,7 +1248,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>94</v>
       </c>
@@ -1197,7 +1259,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>96</v>
       </c>
@@ -1207,8 +1269,14 @@
       <c r="C47" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D47" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E47" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>84</v>
       </c>
@@ -1217,6 +1285,52 @@
       </c>
       <c r="C48" t="s">
         <v>83</v>
+      </c>
+      <c r="D48" t="s">
+        <v>99</v>
+      </c>
+      <c r="E48" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>101</v>
+      </c>
+      <c r="B49">
+        <v>2</v>
+      </c>
+      <c r="C49" t="s">
+        <v>3</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="G49" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>102</v>
+      </c>
+      <c r="B50">
+        <v>8</v>
+      </c>
+      <c r="C50" t="s">
+        <v>35</v>
+      </c>
+      <c r="D50" t="s">
+        <v>108</v>
+      </c>
+      <c r="E50" t="s">
+        <v>109</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="G50" t="s">
+        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>